<commit_message>
update christi data binding
</commit_message>
<xml_diff>
--- a/Data Binding Christi.xlsx
+++ b/Data Binding Christi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\git\HunterCMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D04A87A2-A94C-41D9-A4D0-417C97565578}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B74B7CBC-B026-4DD9-AD24-032CFB4E0BAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{F650361C-5F20-40B9-8782-3E43AA1F215A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F650361C-5F20-40B9-8782-3E43AA1F215A}"/>
   </bookViews>
   <sheets>
     <sheet name="change password" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="55">
   <si>
     <t>status</t>
   </si>
@@ -198,6 +198,9 @@
   </si>
   <si>
     <t>Liburan Keluarga</t>
+  </si>
+  <si>
+    <t>Password2#</t>
   </si>
 </sst>
 </file>
@@ -581,10 +584,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B950DDD1-E905-4EDB-8889-DE1CEFEB7359}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,7 +637,7 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="F2" t="s">
         <v>9</v>
@@ -660,7 +663,7 @@
         <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="G3" t="s">
         <v>9</v>
@@ -686,7 +689,7 @@
         <v>9</v>
       </c>
       <c r="G4" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="H4" t="s">
         <v>8</v>
@@ -706,10 +709,10 @@
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="F5" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="G5" t="s">
         <v>9</v>
@@ -735,10 +738,10 @@
         <v>9</v>
       </c>
       <c r="F6" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="G6" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="H6" t="s">
         <v>8</v>
@@ -758,16 +761,39 @@
         <v>19</v>
       </c>
       <c r="E7" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="F7" t="s">
         <v>9</v>
       </c>
       <c r="G7" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="H7" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -924,7 +950,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E51D11E-B6EF-4BE8-9205-D8027414F64E}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>

</xml_diff>